<commit_message>
Updated the Semi_final files
</commit_message>
<xml_diff>
--- a/Financial_Data/MoneyControl/Companies/IT Services & Consulting/Alphalogic Techsys Ltd/Pruned_Excel/Semi_Final/Alphalogic Techsys Ltd_Semi_Semi_Final.xlsx
+++ b/Financial_Data/MoneyControl/Companies/IT Services & Consulting/Alphalogic Techsys Ltd/Pruned_Excel/Semi_Final/Alphalogic Techsys Ltd_Semi_Semi_Final.xlsx
@@ -18,11 +18,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="87">
   <si>
     <t>Balance Sheet of Alphalogic Techsys(in Rs. Cr.)</t>
   </si>
   <si>
+    <t>Month</t>
+  </si>
+  <si>
     <t>Total share capital</t>
   </si>
   <si>
@@ -59,21 +62,6 @@
     <t>Total assets</t>
   </si>
   <si>
-    <t>Mar 20</t>
-  </si>
-  <si>
-    <t>Mar 21</t>
-  </si>
-  <si>
-    <t>Mar 22</t>
-  </si>
-  <si>
-    <t>Mar 23</t>
-  </si>
-  <si>
-    <t>Mar 24</t>
-  </si>
-  <si>
     <t>Cash Flow of Alphalogic Techsys(in Rs. Cr.)</t>
   </si>
   <si>
@@ -170,6 +158,9 @@
     <t>Quarterly Results of Alphalogic Techsys(in Rs. Cr.)</t>
   </si>
   <si>
+    <t>Quarter</t>
+  </si>
+  <si>
     <t>Net sales/income from operations</t>
   </si>
   <si>
@@ -224,34 +215,16 @@
     <t>Diluted eps.</t>
   </si>
   <si>
-    <t>Jun 22 Q1</t>
-  </si>
-  <si>
-    <t>Sep 22 Q2</t>
-  </si>
-  <si>
-    <t>Dec 22 Q3</t>
-  </si>
-  <si>
-    <t>Mar 23 Q4</t>
-  </si>
-  <si>
-    <t>Jun 23 Q1</t>
-  </si>
-  <si>
-    <t>Sep 23 Q2</t>
-  </si>
-  <si>
-    <t>Dec 23 Q3</t>
-  </si>
-  <si>
-    <t>Mar 24 Q4</t>
-  </si>
-  <si>
-    <t>Jun 24 Q1</t>
-  </si>
-  <si>
-    <t>Sep 24 Q2</t>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
   </si>
   <si>
     <t>Key Financial Ratios of Alphalogic Techsys(in Rs. Cr.)</t>
@@ -663,13 +636,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -709,209 +682,227 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2">
+        <v>2020</v>
+      </c>
       <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
         <v>2.78</v>
-      </c>
-      <c r="C2">
-        <v>7.42</v>
       </c>
       <c r="D2">
         <v>7.42</v>
       </c>
       <c r="E2">
+        <v>7.42</v>
+      </c>
+      <c r="F2">
         <v>10.19</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.05</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>3.81</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>14</v>
-      </c>
-      <c r="I2">
-        <v>0.12</v>
       </c>
       <c r="J2">
         <v>0.12</v>
       </c>
       <c r="K2">
+        <v>0.12</v>
+      </c>
+      <c r="L2">
         <v>9.199999999999999</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>4.8</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
-      <c r="A3" t="s">
-        <v>14</v>
+    <row r="3" spans="1:14">
+      <c r="A3">
+        <v>2021</v>
       </c>
       <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
         <v>2.78</v>
-      </c>
-      <c r="C3">
-        <v>8.01</v>
       </c>
       <c r="D3">
         <v>8.01</v>
       </c>
       <c r="E3">
+        <v>8.01</v>
+      </c>
+      <c r="F3">
         <v>10.78</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.02</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>2.66</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>13.44</v>
-      </c>
-      <c r="I3">
-        <v>0.09</v>
       </c>
       <c r="J3">
         <v>0.09</v>
       </c>
       <c r="K3">
+        <v>0.09</v>
+      </c>
+      <c r="L3">
         <v>10.08</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>3.36</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>13.44</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
-        <v>15</v>
+    <row r="4" spans="1:14">
+      <c r="A4">
+        <v>2022</v>
       </c>
       <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
         <v>11.29</v>
-      </c>
-      <c r="C4">
-        <v>6.64</v>
       </c>
       <c r="D4">
         <v>6.64</v>
       </c>
       <c r="E4">
+        <v>6.64</v>
+      </c>
+      <c r="F4">
         <v>17.93</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.19</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>2.12</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>20.88</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.06</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>2.86</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>19.99</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>0.88</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>20.88</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
-      <c r="A5" t="s">
-        <v>16</v>
+    <row r="5" spans="1:14">
+      <c r="A5">
+        <v>2023</v>
       </c>
       <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
         <v>17.57</v>
-      </c>
-      <c r="C5">
-        <v>6.84</v>
       </c>
       <c r="D5">
         <v>6.84</v>
       </c>
       <c r="E5">
+        <v>6.84</v>
+      </c>
+      <c r="F5">
         <v>24.41</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.07000000000000001</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>4.97</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>30.69</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.04</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>3.49</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>30.01</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>0.68</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>30.69</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
-      <c r="A6" t="s">
-        <v>17</v>
+    <row r="6" spans="1:14">
+      <c r="A6">
+        <v>2024</v>
       </c>
       <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
         <v>23.73</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
       </c>
       <c r="D6">
         <v>7</v>
       </c>
       <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
         <v>30.73</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0.08</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>3.94</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>35.52</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>0.03</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>6.61</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>10.89</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>24.63</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>35.52</v>
       </c>
     </row>
@@ -922,183 +913,201 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>13</v>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2">
+        <v>2020</v>
       </c>
       <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
         <v>2.65</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>-1.68</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>-5.77</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>7.02</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
       <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>-0.44</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.44</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>14</v>
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <v>2021</v>
       </c>
       <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
         <v>0.83</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>2.35</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>-1.24</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>-1.11</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="I3">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>15</v>
+      <c r="J3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>2022</v>
       </c>
       <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
         <v>2.27</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>-4.41</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>-1.84</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>6.25</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>16</v>
+      <c r="J4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>2023</v>
       </c>
       <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
         <v>2.54</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>-6.4</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>-1.92</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>8.32</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
         <v>0.118</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>17</v>
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>2024</v>
       </c>
       <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
         <v>3.88</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>3.47</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>-3.08</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>-0.4</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
         <v>0.01</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>0.01</v>
       </c>
     </row>
@@ -1109,86 +1118,89 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22">
-      <c r="A2" t="s">
-        <v>13</v>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2">
+        <v>2020</v>
       </c>
       <c r="B2">
-        <v>4.68</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>4.68</v>
@@ -1197,46 +1209,46 @@
         <v>4.68</v>
       </c>
       <c r="E2">
+        <v>4.68</v>
+      </c>
+      <c r="F2">
         <v>0.79</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>5.47</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>1.26</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.8</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.17</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>0.02</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>0.58</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>2.82</v>
-      </c>
-      <c r="M2">
-        <v>2.65</v>
       </c>
       <c r="N2">
         <v>2.65</v>
       </c>
       <c r="O2">
+        <v>2.65</v>
+      </c>
+      <c r="P2">
         <v>0.64</v>
       </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
       <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
         <v>0.64</v>
-      </c>
-      <c r="R2">
-        <v>2.01</v>
       </c>
       <c r="S2">
         <v>2.01</v>
@@ -1245,18 +1257,21 @@
         <v>2.01</v>
       </c>
       <c r="U2">
-        <v>9.880000000000001</v>
+        <v>2.01</v>
       </c>
       <c r="V2">
         <v>9.880000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:22">
-      <c r="A3" t="s">
-        <v>14</v>
+      <c r="W2">
+        <v>9.880000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3">
+        <v>2021</v>
       </c>
       <c r="B3">
-        <v>1.8</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>1.8</v>
@@ -1265,46 +1280,46 @@
         <v>1.8</v>
       </c>
       <c r="E3">
+        <v>1.8</v>
+      </c>
+      <c r="F3">
         <v>1.27</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>3.08</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.86</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.36</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.39</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>0.04</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>0.59</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>2.24</v>
-      </c>
-      <c r="M3">
-        <v>0.83</v>
       </c>
       <c r="N3">
         <v>0.83</v>
       </c>
       <c r="O3">
+        <v>0.83</v>
+      </c>
+      <c r="P3">
         <v>0.24</v>
       </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
       <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
         <v>0.24</v>
-      </c>
-      <c r="R3">
-        <v>0.59</v>
       </c>
       <c r="S3">
         <v>0.59</v>
@@ -1313,18 +1328,21 @@
         <v>0.59</v>
       </c>
       <c r="U3">
-        <v>2.14</v>
+        <v>0.59</v>
       </c>
       <c r="V3">
         <v>2.14</v>
       </c>
-    </row>
-    <row r="4" spans="1:22">
-      <c r="A4" t="s">
-        <v>15</v>
+      <c r="W3">
+        <v>2.14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4">
+        <v>2022</v>
       </c>
       <c r="B4">
-        <v>2.84</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>2.84</v>
@@ -1333,46 +1351,46 @@
         <v>2.84</v>
       </c>
       <c r="E4">
+        <v>2.84</v>
+      </c>
+      <c r="F4">
         <v>2.02</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>4.86</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>1.13</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.19</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.5600000000000001</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>0.03</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>0.68</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>2.59</v>
-      </c>
-      <c r="M4">
-        <v>2.27</v>
       </c>
       <c r="N4">
         <v>2.27</v>
       </c>
       <c r="O4">
+        <v>2.27</v>
+      </c>
+      <c r="P4">
         <v>0.54</v>
       </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
       <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
         <v>0.54</v>
-      </c>
-      <c r="R4">
-        <v>1.73</v>
       </c>
       <c r="S4">
         <v>1.73</v>
@@ -1381,18 +1399,21 @@
         <v>1.73</v>
       </c>
       <c r="U4">
-        <v>0.83</v>
+        <v>1.73</v>
       </c>
       <c r="V4">
         <v>0.83</v>
       </c>
-    </row>
-    <row r="5" spans="1:22">
-      <c r="A5" t="s">
-        <v>16</v>
+      <c r="W4">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="A5">
+        <v>2023</v>
       </c>
       <c r="B5">
-        <v>4.35</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>4.35</v>
@@ -1401,46 +1422,46 @@
         <v>4.35</v>
       </c>
       <c r="E5">
+        <v>4.35</v>
+      </c>
+      <c r="F5">
         <v>0.68</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>5.04</v>
       </c>
-      <c r="G5">
-        <v>1.083</v>
-      </c>
       <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
         <v>0.32</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.28</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>0.03</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>1.87</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>2.5</v>
-      </c>
-      <c r="M5">
-        <v>2.54</v>
       </c>
       <c r="N5">
         <v>2.54</v>
       </c>
       <c r="O5">
+        <v>2.54</v>
+      </c>
+      <c r="P5">
         <v>0.66</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>-0.01</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>0.65</v>
-      </c>
-      <c r="R5">
-        <v>1.89</v>
       </c>
       <c r="S5">
         <v>1.89</v>
@@ -1449,18 +1470,21 @@
         <v>1.89</v>
       </c>
       <c r="U5">
+        <v>1.89</v>
+      </c>
+      <c r="V5">
         <v>0.5600000000000001</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>0.55</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
-      <c r="A6" t="s">
-        <v>17</v>
+    <row r="6" spans="1:23">
+      <c r="A6">
+        <v>2024</v>
       </c>
       <c r="B6">
-        <v>6.74</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>6.74</v>
@@ -1469,46 +1493,46 @@
         <v>6.74</v>
       </c>
       <c r="E6">
+        <v>6.74</v>
+      </c>
+      <c r="F6">
         <v>1.01</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>7.75</v>
       </c>
-      <c r="G6">
-        <v>1.083</v>
-      </c>
       <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
         <v>0.36</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>0.46</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>0.01</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>1.37</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>3.87</v>
-      </c>
-      <c r="M6">
-        <v>3.88</v>
       </c>
       <c r="N6">
         <v>3.88</v>
       </c>
       <c r="O6">
+        <v>3.88</v>
+      </c>
+      <c r="P6">
         <v>0.95</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>-0.01</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>0.9399999999999999</v>
-      </c>
-      <c r="R6">
-        <v>2.94</v>
       </c>
       <c r="S6">
         <v>2.94</v>
@@ -1517,9 +1541,12 @@
         <v>2.94</v>
       </c>
       <c r="U6">
+        <v>2.94</v>
+      </c>
+      <c r="V6">
         <v>0.62</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>0.61</v>
       </c>
     </row>
@@ -1530,134 +1557,140 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U11"/>
+  <dimension ref="A1:W11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="S1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2">
+        <v>2022</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>65</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
-      <c r="A2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2">
+      <c r="D2">
         <v>0.9399999999999999</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>0.9399999999999999</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>0.08</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>0.01</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>0.45</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>0.41</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>0.19</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>0.6</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>0.08</v>
-      </c>
-      <c r="K2">
-        <v>0.52</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
       </c>
       <c r="M2">
         <v>0.52</v>
       </c>
       <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0.52</v>
+      </c>
+      <c r="P2">
         <v>0.12</v>
       </c>
-      <c r="O2">
+      <c r="Q2">
         <v>0.4</v>
       </c>
-      <c r="P2">
+      <c r="R2">
         <v>0.4</v>
       </c>
-      <c r="Q2">
+      <c r="S2">
         <v>11.29</v>
-      </c>
-      <c r="R2">
-        <v>0.18</v>
-      </c>
-      <c r="S2">
-        <v>0.18</v>
       </c>
       <c r="T2">
         <v>0.18</v>
@@ -1665,64 +1698,70 @@
       <c r="U2">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="3" spans="1:21">
-      <c r="A3" t="s">
-        <v>69</v>
+      <c r="V2">
+        <v>0.18</v>
+      </c>
+      <c r="W2">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3">
+        <v>2022</v>
       </c>
       <c r="B3">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3">
         <v>1.05</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>1.05</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>0.08</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>0.01</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>0.54</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>0.43</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>0.16</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>0.59</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>0.04</v>
-      </c>
-      <c r="K3">
-        <v>0.55</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
       </c>
       <c r="M3">
         <v>0.55</v>
       </c>
       <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0.55</v>
+      </c>
+      <c r="P3">
         <v>0.14</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>0.41</v>
       </c>
-      <c r="P3">
+      <c r="R3">
         <v>0.41</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <v>16.93</v>
-      </c>
-      <c r="R3">
-        <v>0.12</v>
-      </c>
-      <c r="S3">
-        <v>0.12</v>
       </c>
       <c r="T3">
         <v>0.12</v>
@@ -1730,64 +1769,70 @@
       <c r="U3">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="4" spans="1:21">
-      <c r="A4" t="s">
-        <v>70</v>
+      <c r="V3">
+        <v>0.12</v>
+      </c>
+      <c r="W3">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4">
+        <v>2022</v>
       </c>
       <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4">
         <v>1.07</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>1.07</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>0.07000000000000001</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>0.01</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>0.38</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>0.62</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>0.21</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>0.83</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>0.08</v>
-      </c>
-      <c r="K4">
-        <v>0.75</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
       </c>
       <c r="M4">
         <v>0.75</v>
       </c>
       <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0.75</v>
+      </c>
+      <c r="P4">
         <v>0.2</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>0.55</v>
       </c>
-      <c r="P4">
+      <c r="R4">
         <v>0.55</v>
       </c>
-      <c r="Q4">
+      <c r="S4">
         <v>17.57</v>
-      </c>
-      <c r="R4">
-        <v>0.16</v>
-      </c>
-      <c r="S4">
-        <v>0.16</v>
       </c>
       <c r="T4">
         <v>0.16</v>
@@ -1795,64 +1840,70 @@
       <c r="U4">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="5" spans="1:21">
-      <c r="A5" t="s">
-        <v>71</v>
+      <c r="V4">
+        <v>0.16</v>
+      </c>
+      <c r="W4">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="A5">
+        <v>2023</v>
       </c>
       <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5">
         <v>1.29</v>
       </c>
-      <c r="C5">
+      <c r="E5">
         <v>1.29</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>0.1</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
         <v>0.51</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>0.67</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>0.12</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>0.8</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>0.08</v>
-      </c>
-      <c r="K5">
-        <v>0.72</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
       </c>
       <c r="M5">
         <v>0.72</v>
       </c>
       <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0.72</v>
+      </c>
+      <c r="P5">
         <v>0.19</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
         <v>0.53</v>
       </c>
-      <c r="P5">
+      <c r="R5">
         <v>0.53</v>
       </c>
-      <c r="Q5">
+      <c r="S5">
         <v>17.57</v>
-      </c>
-      <c r="R5">
-        <v>0.16</v>
-      </c>
-      <c r="S5">
-        <v>0.15</v>
       </c>
       <c r="T5">
         <v>0.16</v>
@@ -1860,64 +1911,70 @@
       <c r="U5">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="6" spans="1:21">
-      <c r="A6" t="s">
-        <v>72</v>
+      <c r="V5">
+        <v>0.16</v>
+      </c>
+      <c r="W5">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
+      <c r="A6">
+        <v>2023</v>
       </c>
       <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6">
         <v>1.15</v>
       </c>
-      <c r="C6">
+      <c r="E6">
         <v>1.15</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>0.08</v>
       </c>
-      <c r="E6">
-        <v>0.01</v>
-      </c>
-      <c r="F6">
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>0.31</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>0.75</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>0.17</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>0.93</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>0.08</v>
-      </c>
-      <c r="K6">
-        <v>0.85</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
       </c>
       <c r="M6">
         <v>0.85</v>
       </c>
       <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0.85</v>
+      </c>
+      <c r="P6">
         <v>0.21</v>
       </c>
-      <c r="O6">
+      <c r="Q6">
         <v>0.64</v>
       </c>
-      <c r="P6">
+      <c r="R6">
         <v>0.64</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <v>17.57</v>
-      </c>
-      <c r="R6">
-        <v>0.18</v>
-      </c>
-      <c r="S6">
-        <v>0.18</v>
       </c>
       <c r="T6">
         <v>0.18</v>
@@ -1925,64 +1982,70 @@
       <c r="U6">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="7" spans="1:21">
-      <c r="A7" t="s">
-        <v>73</v>
+      <c r="V6">
+        <v>0.18</v>
+      </c>
+      <c r="W6">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="A7">
+        <v>2023</v>
       </c>
       <c r="B7">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7">
         <v>1.26</v>
       </c>
-      <c r="C7">
+      <c r="E7">
         <v>1.26</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>0.08</v>
       </c>
-      <c r="E7">
-        <v>0.01</v>
-      </c>
-      <c r="F7">
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>0.31</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>0.86</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>0.29</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>1.15</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>0.11</v>
-      </c>
-      <c r="K7">
-        <v>1.04</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
       </c>
       <c r="M7">
         <v>1.04</v>
       </c>
       <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>1.04</v>
+      </c>
+      <c r="P7">
         <v>0.26</v>
       </c>
-      <c r="O7">
+      <c r="Q7">
         <v>0.77</v>
       </c>
-      <c r="P7">
+      <c r="R7">
         <v>0.77</v>
       </c>
-      <c r="Q7">
+      <c r="S7">
         <v>17.57</v>
-      </c>
-      <c r="R7">
-        <v>0.22</v>
-      </c>
-      <c r="S7">
-        <v>0.21</v>
       </c>
       <c r="T7">
         <v>0.22</v>
@@ -1990,64 +2053,70 @@
       <c r="U7">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="8" spans="1:21">
-      <c r="A8" t="s">
-        <v>74</v>
+      <c r="V7">
+        <v>0.22</v>
+      </c>
+      <c r="W7">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8">
+        <v>2023</v>
       </c>
       <c r="B8">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8">
         <v>1.16</v>
       </c>
-      <c r="C8">
+      <c r="E8">
         <v>1.16</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>0.1</v>
       </c>
-      <c r="E8">
-        <v>0.01</v>
-      </c>
-      <c r="F8">
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
         <v>0.41</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>0.64</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>0.47</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>1.11</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>0.15</v>
-      </c>
-      <c r="K8">
-        <v>0.96</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
       </c>
       <c r="M8">
         <v>0.96</v>
       </c>
       <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0.96</v>
+      </c>
+      <c r="P8">
         <v>0.21</v>
       </c>
-      <c r="O8">
+      <c r="Q8">
         <v>0.74</v>
       </c>
-      <c r="P8">
+      <c r="R8">
         <v>0.74</v>
       </c>
-      <c r="Q8">
+      <c r="S8">
         <v>23.43</v>
-      </c>
-      <c r="R8">
-        <v>0.16</v>
-      </c>
-      <c r="S8">
-        <v>0.15</v>
       </c>
       <c r="T8">
         <v>0.16</v>
@@ -2055,64 +2124,70 @@
       <c r="U8">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="9" spans="1:21">
-      <c r="A9" t="s">
-        <v>75</v>
+      <c r="V8">
+        <v>0.16</v>
+      </c>
+      <c r="W8">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="A9">
+        <v>2024</v>
       </c>
       <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9">
         <v>3.17</v>
       </c>
-      <c r="C9">
+      <c r="E9">
         <v>3.17</v>
       </c>
-      <c r="D9">
+      <c r="F9">
         <v>0.09</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
         <v>0.33</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>1.07</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>0.08</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>1.15</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>0.12</v>
-      </c>
-      <c r="K9">
-        <v>1.03</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
       </c>
       <c r="M9">
         <v>1.03</v>
       </c>
       <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>1.03</v>
+      </c>
+      <c r="P9">
         <v>0.25</v>
       </c>
-      <c r="O9">
+      <c r="Q9">
         <v>0.78</v>
       </c>
-      <c r="P9">
+      <c r="R9">
         <v>0.78</v>
       </c>
-      <c r="Q9">
+      <c r="S9">
         <v>23.73</v>
-      </c>
-      <c r="R9">
-        <v>0.17</v>
-      </c>
-      <c r="S9">
-        <v>0.16</v>
       </c>
       <c r="T9">
         <v>0.17</v>
@@ -2120,64 +2195,70 @@
       <c r="U9">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="10" spans="1:21">
-      <c r="A10" t="s">
-        <v>76</v>
+      <c r="V9">
+        <v>0.17</v>
+      </c>
+      <c r="W9">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10">
+        <v>2024</v>
       </c>
       <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10">
         <v>1.97</v>
       </c>
-      <c r="C10">
+      <c r="E10">
         <v>1.97</v>
       </c>
-      <c r="D10">
+      <c r="F10">
         <v>0.09</v>
       </c>
-      <c r="E10">
-        <v>0.01</v>
-      </c>
-      <c r="F10">
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>0.26</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>0.89</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>0.24</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>1.13</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>0.05</v>
-      </c>
-      <c r="K10">
-        <v>1.07</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
       </c>
       <c r="M10">
         <v>1.07</v>
       </c>
       <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>1.07</v>
+      </c>
+      <c r="P10">
         <v>0.26</v>
       </c>
-      <c r="O10">
+      <c r="Q10">
         <v>0.8100000000000001</v>
       </c>
-      <c r="P10">
+      <c r="R10">
         <v>0.8100000000000001</v>
       </c>
-      <c r="Q10">
+      <c r="S10">
         <v>24.24</v>
-      </c>
-      <c r="R10">
-        <v>0.17</v>
-      </c>
-      <c r="S10">
-        <v>0.17</v>
       </c>
       <c r="T10">
         <v>0.17</v>
@@ -2185,69 +2266,81 @@
       <c r="U10">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="11" spans="1:21">
-      <c r="A11" t="s">
-        <v>77</v>
+      <c r="V10">
+        <v>0.17</v>
+      </c>
+      <c r="W10">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
+      <c r="A11">
+        <v>2024</v>
       </c>
       <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11">
         <v>1.51</v>
       </c>
-      <c r="C11">
+      <c r="E11">
         <v>1.51</v>
       </c>
-      <c r="D11">
+      <c r="F11">
         <v>0.08</v>
       </c>
-      <c r="E11">
-        <v>0.01</v>
-      </c>
-      <c r="F11">
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
         <v>0.28</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <v>0.63</v>
       </c>
-      <c r="H11">
+      <c r="J11">
         <v>0.51</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <v>1.15</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>0.07000000000000001</v>
-      </c>
-      <c r="K11">
-        <v>1.07</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
       </c>
       <c r="M11">
         <v>1.07</v>
       </c>
       <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>1.07</v>
+      </c>
+      <c r="P11">
         <v>0.28</v>
       </c>
-      <c r="O11">
+      <c r="Q11">
         <v>0.8</v>
       </c>
-      <c r="P11">
+      <c r="R11">
         <v>0.8</v>
       </c>
-      <c r="Q11">
+      <c r="S11">
         <v>31.31</v>
-      </c>
-      <c r="R11">
-        <v>0.13</v>
-      </c>
-      <c r="S11">
-        <v>0.13</v>
       </c>
       <c r="T11">
         <v>0.13</v>
       </c>
       <c r="U11">
+        <v>0.13</v>
+      </c>
+      <c r="V11">
+        <v>0.13</v>
+      </c>
+      <c r="W11">
         <v>0.13</v>
       </c>
     </row>
@@ -2258,111 +2351,114 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
-      <c r="A2" t="s">
-        <v>13</v>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2">
+        <v>2020</v>
       </c>
       <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
         <v>16.86</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>10.23</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>10.15</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>9.539999999999999</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>7.24</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>60.64</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>60.18</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>56.57</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>42.94</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>19.72</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>14.35</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>0.24</v>
       </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
       <c r="O2">
         <v>0</v>
       </c>
@@ -2370,55 +2466,58 @@
         <v>0</v>
       </c>
       <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
         <v>26.02</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>9.17</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
-      <c r="A3" t="s">
-        <v>14</v>
+    <row r="3" spans="1:19">
+      <c r="A3">
+        <v>2021</v>
       </c>
       <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
         <v>6.49</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>4.54</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>4.42</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>3</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>2.14</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>69.97</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>67.98999999999999</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>46.21</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>32.88</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>5.49</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>4.4</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>0.16</v>
       </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
       <c r="O3">
         <v>0</v>
       </c>
@@ -2426,55 +2525,58 @@
         <v>0</v>
       </c>
       <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
         <v>25.36</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>20.1</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
-      <c r="A4" t="s">
-        <v>15</v>
+    <row r="4" spans="1:19">
+      <c r="A4">
+        <v>2022</v>
       </c>
       <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
         <v>1.26</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>1.27</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>1.25</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>1.01</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.77</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>100.71</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>99.61</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>79.87</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>60.96</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>9.65</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>8.289999999999999</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>0.15</v>
       </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
       <c r="O4">
         <v>0</v>
       </c>
@@ -2482,55 +2584,58 @@
         <v>0</v>
       </c>
       <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
         <v>84.67</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>29.6</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
-      <c r="A5" t="s">
-        <v>16</v>
+    <row r="5" spans="1:19">
+      <c r="A5">
+        <v>2023</v>
       </c>
       <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
         <v>1.24</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>0.8100000000000001</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0.8</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0.72</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.54</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>65.33</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>64.73</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>58.32</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>43.41</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>7.74</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>6.15</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>0.19</v>
       </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
       <c r="O5">
         <v>0</v>
       </c>
@@ -2538,55 +2643,58 @@
         <v>0</v>
       </c>
       <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
         <v>117.56</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>41.32</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
-      <c r="A6" t="s">
-        <v>17</v>
+    <row r="6" spans="1:19">
+      <c r="A6">
+        <v>2024</v>
       </c>
       <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
         <v>1.42</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>0.92</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0.91</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>0.82</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0.62</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>64.59</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>64.42</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>57.55</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>43.64</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>9.56</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>8.27</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>0.11</v>
       </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
       <c r="O6">
         <v>0</v>
       </c>
@@ -2594,9 +2702,12 @@
         <v>0</v>
       </c>
       <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
         <v>380.17</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>87.38</v>
       </c>
     </row>

</xml_diff>